<commit_message>
1. Add react component: SitePlan. 2. Minor changes. 3. Bugfix.
</commit_message>
<xml_diff>
--- a/django_backend/var/sys/views/core/TypeWidgetMnt-v0.xlsx
+++ b/django_backend/var/sys/views/core/TypeWidgetMnt-v0.xlsx
@@ -637,7 +637,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -841,7 +847,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -876,7 +881,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1060,1560 +1064,1580 @@
   <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18.28515625" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="26" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="23.140625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="23.85546875" customWidth="1" min="5" max="5"/>
-    <col width="16.42578125" customWidth="1" min="6" max="8"/>
-    <col width="20.5703125" customWidth="1" min="9" max="9"/>
-    <col width="18.5703125" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="18.42578125" customWidth="1" min="11" max="11"/>
-    <col width="23.140625" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="16" bestFit="1" customWidth="1" min="13" max="13"/>
-    <col width="26.85546875" customWidth="1" min="14" max="14"/>
-    <col width="23.5703125" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="17" bestFit="1" customWidth="1" min="16" max="16"/>
-    <col width="23.140625" bestFit="1" customWidth="1" min="17" max="17"/>
-    <col width="11.7109375" customWidth="1" min="18" max="18"/>
-    <col width="10.7109375" bestFit="1" customWidth="1" min="19" max="19"/>
-    <col width="22.42578125" bestFit="1" customWidth="1" min="20" max="20"/>
-    <col width="10" bestFit="1" customWidth="1" min="21" max="21"/>
-    <col width="10" customWidth="1" min="22" max="26"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" min="27" max="27"/>
-    <col width="13.5703125" customWidth="1" min="28" max="30"/>
+    <col width="18.28515625" customWidth="1" style="11" min="1" max="1"/>
+    <col width="13" customWidth="1" style="4" min="2" max="2"/>
+    <col width="26" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="23.140625" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
+    <col width="23.85546875" customWidth="1" style="4" min="5" max="5"/>
+    <col width="16.42578125" customWidth="1" style="4" min="6" max="8"/>
+    <col width="20.5703125" customWidth="1" style="4" min="9" max="9"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" style="4" min="10" max="10"/>
+    <col width="18.42578125" customWidth="1" style="4" min="11" max="11"/>
+    <col width="23.140625" bestFit="1" customWidth="1" style="4" min="12" max="12"/>
+    <col width="16" bestFit="1" customWidth="1" style="4" min="13" max="13"/>
+    <col width="26.85546875" customWidth="1" style="4" min="14" max="14"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" style="4" min="15" max="15"/>
+    <col width="17" bestFit="1" customWidth="1" style="4" min="16" max="16"/>
+    <col width="23.140625" bestFit="1" customWidth="1" style="4" min="17" max="17"/>
+    <col width="11.7109375" customWidth="1" style="4" min="18" max="18"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" style="4" min="19" max="19"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" style="4" min="20" max="20"/>
+    <col width="10" bestFit="1" customWidth="1" style="4" min="21" max="21"/>
+    <col width="10" customWidth="1" style="4" min="22" max="26"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="4" min="27" max="27"/>
+    <col width="13.5703125" customWidth="1" style="4" min="28" max="30"/>
   </cols>
   <sheetData>
-    <row r="1" ht="37.5" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="37.5" customHeight="1" s="4">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Do not modify this column</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Screen Definition - v1</t>
-        </is>
-      </c>
-      <c r="D1" s="8" t="n"/>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Screen Definition - v2</t>
+        </is>
+      </c>
+      <c r="D1" s="12" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="n"/>
+      <c r="A2" s="10" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
         <is>
           <t>viewAPIRev</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>API Version</t>
         </is>
       </c>
-      <c r="C3" s="16" t="n">
+      <c r="C3" s="20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>viewID</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>Screen ID</t>
         </is>
       </c>
-      <c r="C4" s="12" t="inlineStr">
+      <c r="C4" s="16" t="inlineStr">
         <is>
           <t>TypeWidgetMnt</t>
         </is>
       </c>
-      <c r="D4" s="8" t="n"/>
-      <c r="E4" s="8" t="n"/>
+      <c r="D4" s="12" t="n"/>
+      <c r="E4" s="12" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>viewTitle</t>
         </is>
       </c>
-      <c r="B5" s="1" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Screen Title</t>
         </is>
       </c>
-      <c r="C5" s="12" t="inlineStr">
+      <c r="C5" s="16" t="inlineStr">
         <is>
           <t>Field Group Type and Field Widget Management</t>
         </is>
       </c>
-      <c r="D5" s="8" t="n"/>
-      <c r="E5" s="8" t="n"/>
+      <c r="D5" s="12" t="n"/>
+      <c r="E5" s="12" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="10" t="inlineStr">
         <is>
           <t>viewDesc</t>
         </is>
       </c>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="C6" s="12" t="inlineStr">
+      <c r="C6" s="16" t="inlineStr">
         <is>
           <t>Field Group Type and Field Widget Management</t>
         </is>
       </c>
-      <c r="D6" s="8" t="inlineStr">
+      <c r="D6" s="12" t="inlineStr">
         <is>
           <t>optional</t>
         </is>
       </c>
-      <c r="E6" s="8" t="n"/>
+      <c r="E6" s="12" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>layoutType</t>
         </is>
       </c>
-      <c r="B7" s="1" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>Layout Type</t>
         </is>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="8" t="inlineStr">
+      <c r="D7" s="12" t="inlineStr">
         <is>
           <t>see notes 1</t>
         </is>
       </c>
-      <c r="E7" s="8" t="n"/>
+      <c r="E7" s="12" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>layoutParams</t>
         </is>
       </c>
-      <c r="B8" s="1" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>Layout Parameters</t>
         </is>
       </c>
-      <c r="C8" s="12" t="n"/>
-      <c r="D8" s="8" t="n"/>
-      <c r="E8" s="8" t="n"/>
+      <c r="C8" s="16" t="n"/>
+      <c r="D8" s="12" t="n"/>
+      <c r="E8" s="12" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="10" t="inlineStr">
         <is>
           <t>viewName</t>
         </is>
       </c>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>Class Name</t>
         </is>
       </c>
-      <c r="C9" s="12" t="inlineStr">
+      <c r="C9" s="16" t="inlineStr">
         <is>
           <t>core.views.TypeWidgetMnt</t>
         </is>
       </c>
-      <c r="D9" s="8" t="inlineStr">
+      <c r="D9" s="12" t="inlineStr">
         <is>
           <t>Python / Javascript ClassName</t>
         </is>
       </c>
-      <c r="E9" s="8" t="n"/>
+      <c r="E9" s="12" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>apiUrl</t>
         </is>
       </c>
-      <c r="B10" s="1" t="inlineStr">
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>API URL</t>
         </is>
       </c>
-      <c r="C10" s="12" t="n"/>
-      <c r="D10" s="8" t="n"/>
-      <c r="E10" s="8" t="n"/>
+      <c r="C10" s="16" t="n"/>
+      <c r="D10" s="12" t="n"/>
+      <c r="E10" s="12" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="inlineStr">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>editable</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr">
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>Editable</t>
         </is>
       </c>
-      <c r="C11" s="12" t="inlineStr">
+      <c r="C11" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D11" s="8" t="inlineStr">
+      <c r="D11" s="12" t="inlineStr">
         <is>
           <t>yes/no</t>
         </is>
       </c>
-      <c r="E11" s="8" t="n"/>
+      <c r="E11" s="12" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="inlineStr">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>autoRefresh</t>
         </is>
       </c>
-      <c r="B12" s="1" t="inlineStr">
+      <c r="B12" s="5" t="inlineStr">
         <is>
           <t>Auto Refresh</t>
         </is>
       </c>
-      <c r="C12" s="12" t="n"/>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="C12" s="16" t="n"/>
+      <c r="D12" s="12" t="inlineStr">
         <is>
           <t>Format: Interval[;action]. Interval: second. E.g. "10", "10;Search"</t>
         </is>
       </c>
-      <c r="E12" s="8" t="n"/>
+      <c r="E12" s="12" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="inlineStr">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>rev</t>
         </is>
       </c>
-      <c r="B13" s="1" t="inlineStr">
+      <c r="B13" s="5" t="inlineStr">
         <is>
           <t>Reversion</t>
         </is>
       </c>
-      <c r="C13" s="12" t="n">
+      <c r="C13" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D13" s="8" t="inlineStr">
+      <c r="D13" s="12" t="inlineStr">
         <is>
           <t>0, 1, 2 …</t>
         </is>
       </c>
-      <c r="E13" s="8" t="n"/>
+      <c r="E13" s="12" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="inlineStr">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>rmk</t>
         </is>
       </c>
-      <c r="B14" s="1" t="inlineStr">
+      <c r="B14" s="5" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
-      <c r="C14" s="12" t="n"/>
-      <c r="D14" s="8" t="n"/>
-      <c r="E14" s="8" t="n"/>
+      <c r="C14" s="16" t="n"/>
+      <c r="D14" s="12" t="n"/>
+      <c r="E14" s="12" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="n"/>
-      <c r="I15" s="9" t="n"/>
-      <c r="N15" s="9" t="n"/>
-      <c r="O15" s="9" t="n"/>
+      <c r="A15" s="10" t="n"/>
+      <c r="I15" s="13" t="n"/>
+      <c r="N15" s="13" t="n"/>
+      <c r="O15" s="13" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="n"/>
-      <c r="C16" s="9" t="inlineStr">
+      <c r="A16" s="10" t="n"/>
+      <c r="C16" s="13" t="inlineStr">
         <is>
           <t>Python Name / View Name</t>
         </is>
       </c>
-      <c r="D16" s="9" t="inlineStr">
+      <c r="D16" s="13" t="inlineStr">
         <is>
           <t>SQL</t>
         </is>
       </c>
-      <c r="F16" s="9" t="n"/>
-      <c r="N16" s="9" t="n"/>
-      <c r="O16" s="9" t="n"/>
-      <c r="Q16" s="9" t="n"/>
-      <c r="R16" s="9" t="n"/>
+      <c r="F16" s="13" t="n"/>
+      <c r="N16" s="13" t="n"/>
+      <c r="O16" s="13" t="n"/>
+      <c r="Q16" s="13" t="n"/>
+      <c r="R16" s="13" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="inlineStr">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>recordsetTable</t>
         </is>
       </c>
-      <c r="B17" s="1" t="inlineStr">
+      <c r="B17" s="5" t="inlineStr">
         <is>
           <t>Recordset</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
+      <c r="C17" s="7" t="inlineStr">
         <is>
           <t>Recordset Name</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr">
+      <c r="D17" s="7" t="inlineStr">
         <is>
           <t>Select Fields</t>
         </is>
       </c>
-      <c r="E17" s="3" t="inlineStr">
+      <c r="E17" s="7" t="inlineStr">
         <is>
           <t>Models</t>
         </is>
       </c>
-      <c r="F17" s="3" t="inlineStr">
+      <c r="F17" s="7" t="inlineStr">
         <is>
           <t>Where</t>
         </is>
       </c>
-      <c r="G17" s="3" t="inlineStr">
+      <c r="G17" s="7" t="inlineStr">
         <is>
           <t>Order</t>
         </is>
       </c>
-      <c r="H17" s="3" t="inlineStr">
+      <c r="H17" s="7" t="inlineStr">
         <is>
           <t>Limit</t>
         </is>
       </c>
-      <c r="I17" s="3" t="inlineStr">
+      <c r="I17" s="7" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="n"/>
-      <c r="C18" s="12" t="inlineStr">
+      <c r="A18" s="10" t="n"/>
+      <c r="C18" s="16" t="inlineStr">
         <is>
           <t>customFgTypeRcs</t>
         </is>
       </c>
-      <c r="D18" s="12" t="inlineStr">
+      <c r="D18" s="16" t="inlineStr">
         <is>
           <t>*</t>
         </is>
       </c>
-      <c r="E18" s="12" t="inlineStr">
+      <c r="E18" s="16" t="inlineStr">
         <is>
           <t>core.models.ScreenFgType</t>
         </is>
       </c>
-      <c r="F18" s="12" t="n"/>
-      <c r="G18" s="12" t="n"/>
-      <c r="H18" s="12" t="n"/>
-      <c r="I18" s="12" t="n"/>
+      <c r="F18" s="16" t="n"/>
+      <c r="G18" s="16" t="n"/>
+      <c r="H18" s="16" t="n"/>
+      <c r="I18" s="16" t="n"/>
     </row>
     <row r="19">
-      <c r="C19" s="12" t="inlineStr">
+      <c r="C19" s="16" t="inlineStr">
         <is>
           <t>customFieldWidgetRcs</t>
         </is>
       </c>
-      <c r="D19" s="12" t="inlineStr">
+      <c r="D19" s="16" t="inlineStr">
         <is>
           <t>*</t>
         </is>
       </c>
-      <c r="E19" s="12" t="inlineStr">
+      <c r="E19" s="16" t="inlineStr">
         <is>
           <t>core.models.ScreenFieldWidget</t>
         </is>
       </c>
-      <c r="F19" s="12" t="n"/>
-      <c r="G19" s="12" t="n"/>
-      <c r="H19" s="12" t="n"/>
-      <c r="I19" s="12" t="n"/>
+      <c r="F19" s="16" t="n"/>
+      <c r="G19" s="16" t="n"/>
+      <c r="H19" s="16" t="n"/>
+      <c r="I19" s="16" t="n"/>
     </row>
     <row r="20">
-      <c r="C20" s="12" t="inlineStr">
+      <c r="C20" s="16" t="inlineStr">
         <is>
           <t>systemFgTypeRcs</t>
         </is>
       </c>
-      <c r="D20" s="12" t="inlineStr">
+      <c r="D20" s="16" t="inlineStr">
         <is>
           <t>*</t>
         </is>
       </c>
-      <c r="E20" s="12" t="inlineStr">
+      <c r="E20" s="16" t="inlineStr">
         <is>
           <t>core.models.ScreenFgType</t>
         </is>
       </c>
-      <c r="F20" s="12" t="n"/>
-      <c r="G20" s="12" t="n"/>
-      <c r="H20" s="12" t="n"/>
-      <c r="I20" s="12" t="n"/>
+      <c r="F20" s="16" t="n"/>
+      <c r="G20" s="16" t="n"/>
+      <c r="H20" s="16" t="n"/>
+      <c r="I20" s="16" t="n"/>
     </row>
     <row r="21">
-      <c r="C21" s="12" t="inlineStr">
+      <c r="C21" s="16" t="inlineStr">
         <is>
           <t>systemFieldWidgetRcs</t>
         </is>
       </c>
-      <c r="D21" s="12" t="inlineStr">
+      <c r="D21" s="16" t="inlineStr">
         <is>
           <t>*</t>
         </is>
       </c>
-      <c r="E21" s="12" t="inlineStr">
+      <c r="E21" s="16" t="inlineStr">
         <is>
           <t>core.models.ScreenFieldWidget</t>
         </is>
       </c>
-      <c r="F21" s="12" t="n"/>
-      <c r="G21" s="12" t="n"/>
-      <c r="H21" s="12" t="n"/>
-      <c r="I21" s="12" t="n"/>
+      <c r="F21" s="16" t="n"/>
+      <c r="G21" s="16" t="n"/>
+      <c r="H21" s="16" t="n"/>
+      <c r="I21" s="16" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="n"/>
-      <c r="C22" s="5" t="inlineStr">
+      <c r="A22" s="10" t="n"/>
+      <c r="C22" s="9" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D22" s="3" t="n"/>
-      <c r="E22" s="3" t="n"/>
-      <c r="F22" s="3" t="n"/>
-      <c r="G22" s="3" t="n"/>
-      <c r="H22" s="3" t="n"/>
-      <c r="I22" s="3" t="n"/>
+      <c r="D22" s="7" t="n"/>
+      <c r="E22" s="7" t="n"/>
+      <c r="F22" s="7" t="n"/>
+      <c r="G22" s="7" t="n"/>
+      <c r="H22" s="7" t="n"/>
+      <c r="I22" s="7" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="n"/>
+      <c r="A23" s="10" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="n"/>
-      <c r="D24" s="9" t="inlineStr">
+      <c r="A24" s="10" t="n"/>
+      <c r="D24" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">fields, table, </t>
         </is>
       </c>
+      <c r="S24" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Additional Properties optional keys: </t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="n"/>
-      <c r="C25" s="9" t="n"/>
-      <c r="D25" s="9" t="inlineStr">
+      <c r="A25" s="10" t="n"/>
+      <c r="C25" s="13" t="n"/>
+      <c r="D25" s="13" t="inlineStr">
         <is>
           <t>chart, iconBar</t>
         </is>
       </c>
-      <c r="G25" s="9" t="inlineStr">
+      <c r="G25" s="13" t="inlineStr">
         <is>
           <t>( yes/ blank )</t>
         </is>
       </c>
-      <c r="H25" s="9" t="inlineStr">
+      <c r="H25" s="13" t="inlineStr">
         <is>
           <t>( yes/ blank )</t>
         </is>
       </c>
-      <c r="I25" s="9" t="inlineStr">
+      <c r="I25" s="13" t="inlineStr">
         <is>
           <t>( yes/ blank )</t>
         </is>
       </c>
-      <c r="J25" s="9" t="inlineStr">
+      <c r="J25" s="13" t="inlineStr">
         <is>
           <t>( yes/ blank )</t>
         </is>
       </c>
-      <c r="K25" s="9" t="inlineStr">
+      <c r="K25" s="13" t="inlineStr">
         <is>
           <t>( single/ multiple/ blank )</t>
         </is>
       </c>
-      <c r="L25" s="9" t="n"/>
-      <c r="M25" s="9" t="inlineStr">
-        <is>
-          <t>( yes/ blank )</t>
-        </is>
-      </c>
-      <c r="N25" s="9" t="inlineStr">
+      <c r="L25" s="13" t="n"/>
+      <c r="M25" s="13" t="inlineStr">
         <is>
           <t>( client/ server/ blank )</t>
         </is>
       </c>
-      <c r="O25" s="9" t="n"/>
+      <c r="N25" s="13" t="n"/>
+      <c r="S25" s="13" t="inlineStr">
+        <is>
+          <t>sortNewRows / tableHeight / …</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="inlineStr">
+      <c r="A26" s="11" t="inlineStr">
         <is>
           <t>fieldGroupTable</t>
         </is>
       </c>
-      <c r="B26" s="1" t="inlineStr">
+      <c r="B26" s="5" t="inlineStr">
         <is>
           <t>Field Groups</t>
         </is>
       </c>
-      <c r="C26" s="3" t="inlineStr">
+      <c r="C26" s="7" t="inlineStr">
         <is>
           <t>Field Group Name</t>
         </is>
       </c>
-      <c r="D26" s="3" t="inlineStr">
+      <c r="D26" s="7" t="inlineStr">
         <is>
           <t>Group Type</t>
         </is>
       </c>
-      <c r="E26" s="3" t="inlineStr">
+      <c r="E26" s="7" t="inlineStr">
         <is>
           <t>Caption</t>
         </is>
       </c>
-      <c r="F26" s="3" t="inlineStr">
+      <c r="F26" s="7" t="inlineStr">
         <is>
           <t>Recordset</t>
         </is>
       </c>
-      <c r="G26" s="3" t="inlineStr">
+      <c r="G26" s="7" t="inlineStr">
         <is>
           <t>Deletable</t>
         </is>
       </c>
-      <c r="H26" s="3" t="inlineStr">
+      <c r="H26" s="7" t="inlineStr">
         <is>
           <t>Editable</t>
         </is>
       </c>
-      <c r="I26" s="3" t="inlineStr">
+      <c r="I26" s="7" t="inlineStr">
         <is>
           <t>Insertable</t>
         </is>
       </c>
-      <c r="J26" s="3" t="inlineStr">
+      <c r="J26" s="7" t="inlineStr">
         <is>
           <t>Highlight Row</t>
         </is>
       </c>
-      <c r="K26" s="3" t="inlineStr">
+      <c r="K26" s="7" t="inlineStr">
         <is>
           <t>Selection Mode</t>
         </is>
       </c>
-      <c r="L26" s="3" t="inlineStr">
+      <c r="L26" s="7" t="inlineStr">
         <is>
           <t>Cols</t>
         </is>
       </c>
-      <c r="M26" s="3" t="inlineStr">
-        <is>
-          <t>Sort New Rows</t>
-        </is>
-      </c>
-      <c r="N26" s="3" t="inlineStr">
+      <c r="M26" s="7" t="inlineStr">
         <is>
           <t>Page Type</t>
         </is>
       </c>
-      <c r="O26" s="3" t="inlineStr">
+      <c r="N26" s="7" t="inlineStr">
         <is>
           <t>Page Size</t>
         </is>
       </c>
-      <c r="P26" s="3" t="inlineStr">
+      <c r="O26" s="7" t="inlineStr">
         <is>
           <t>Outer Layout Parameters</t>
         </is>
       </c>
-      <c r="Q26" s="3" t="inlineStr">
+      <c r="P26" s="7" t="inlineStr">
         <is>
           <t>Inner Layout Type</t>
         </is>
       </c>
-      <c r="R26" s="3" t="inlineStr">
+      <c r="Q26" s="7" t="inlineStr">
         <is>
           <t>Inner Layout Parameters</t>
         </is>
       </c>
-      <c r="S26" s="3" t="inlineStr">
+      <c r="R26" s="7" t="inlineStr">
         <is>
           <t>Html</t>
         </is>
       </c>
-      <c r="T26" s="3" t="inlineStr">
+      <c r="S26" s="7" t="inlineStr">
+        <is>
+          <t>Additional Properties</t>
+        </is>
+      </c>
+      <c r="T26" s="7" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="12" t="inlineStr">
+      <c r="A27" s="11" t="n"/>
+      <c r="B27" s="5" t="n"/>
+      <c r="C27" s="16" t="inlineStr">
         <is>
           <t>systemFgTypeFg</t>
         </is>
       </c>
-      <c r="D27" s="12" t="inlineStr">
+      <c r="D27" s="16" t="inlineStr">
         <is>
           <t>table</t>
         </is>
       </c>
-      <c r="E27" s="12" t="inlineStr">
+      <c r="E27" s="16" t="inlineStr">
         <is>
           <t>System Field Group Type</t>
         </is>
       </c>
-      <c r="F27" s="12" t="inlineStr">
+      <c r="F27" s="16" t="inlineStr">
         <is>
           <t>systemFgTypeRcs</t>
         </is>
       </c>
-      <c r="G27" s="12" t="inlineStr"/>
-      <c r="H27" s="12" t="inlineStr"/>
-      <c r="I27" s="12" t="inlineStr"/>
-      <c r="J27" s="12" t="inlineStr">
+      <c r="G27" s="16" t="inlineStr"/>
+      <c r="H27" s="16" t="inlineStr"/>
+      <c r="I27" s="16" t="inlineStr"/>
+      <c r="J27" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="K27" s="12" t="n"/>
-      <c r="L27" s="12" t="n"/>
-      <c r="M27" s="12" t="inlineStr"/>
-      <c r="N27" s="12" t="n"/>
-      <c r="O27" s="12" t="n"/>
-      <c r="P27" s="12" t="n"/>
-      <c r="Q27" s="12" t="n"/>
-      <c r="R27" s="12" t="n"/>
-      <c r="S27" s="12" t="n"/>
-      <c r="T27" s="12" t="n"/>
+      <c r="K27" s="16" t="n"/>
+      <c r="L27" s="16" t="n"/>
+      <c r="M27" s="16" t="n"/>
+      <c r="N27" s="16" t="n"/>
+      <c r="O27" s="16" t="n"/>
+      <c r="P27" s="16" t="n"/>
+      <c r="Q27" s="16" t="n"/>
+      <c r="R27" s="16" t="n"/>
+      <c r="S27" s="16" t="n"/>
+      <c r="T27" s="16" t="n"/>
     </row>
     <row r="28">
-      <c r="C28" s="12" t="inlineStr">
+      <c r="C28" s="16" t="inlineStr">
         <is>
           <t>customFgTypeFg</t>
         </is>
       </c>
-      <c r="D28" s="12" t="inlineStr">
+      <c r="D28" s="16" t="inlineStr">
         <is>
           <t>table</t>
         </is>
       </c>
-      <c r="E28" s="12" t="inlineStr">
+      <c r="E28" s="16" t="inlineStr">
         <is>
           <t>Custom Field Group Type</t>
         </is>
       </c>
-      <c r="F28" s="12" t="inlineStr">
+      <c r="F28" s="16" t="inlineStr">
         <is>
           <t>customFgTypeRcs</t>
         </is>
       </c>
-      <c r="G28" s="12" t="inlineStr">
+      <c r="G28" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H28" s="12" t="inlineStr">
+      <c r="H28" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="I28" s="12" t="inlineStr">
+      <c r="I28" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="J28" s="12" t="inlineStr">
+      <c r="J28" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="K28" s="12" t="n"/>
-      <c r="L28" s="12" t="n"/>
-      <c r="M28" s="12" t="inlineStr"/>
-      <c r="N28" s="12" t="n"/>
-      <c r="O28" s="12" t="n"/>
-      <c r="P28" s="12" t="n"/>
-      <c r="Q28" s="12" t="n"/>
-      <c r="R28" s="12" t="n"/>
-      <c r="S28" s="12" t="n"/>
-      <c r="T28" s="12" t="n"/>
+      <c r="K28" s="16" t="n"/>
+      <c r="L28" s="16" t="n"/>
+      <c r="M28" s="16" t="n"/>
+      <c r="N28" s="16" t="n"/>
+      <c r="O28" s="16" t="n"/>
+      <c r="P28" s="16" t="n"/>
+      <c r="Q28" s="16" t="n"/>
+      <c r="R28" s="16" t="n"/>
+      <c r="S28" s="16" t="n"/>
+      <c r="T28" s="16" t="n"/>
     </row>
     <row r="29">
-      <c r="C29" s="12" t="inlineStr">
+      <c r="C29" s="16" t="inlineStr">
         <is>
           <t>fgTypeToolbar</t>
         </is>
       </c>
-      <c r="D29" s="12" t="inlineStr">
+      <c r="D29" s="16" t="inlineStr">
         <is>
           <t>iconBar</t>
         </is>
       </c>
-      <c r="E29" s="12" t="n"/>
-      <c r="F29" s="12" t="n"/>
-      <c r="G29" s="12" t="inlineStr"/>
-      <c r="H29" s="12" t="inlineStr"/>
-      <c r="I29" s="12" t="inlineStr"/>
-      <c r="J29" s="12" t="inlineStr"/>
-      <c r="K29" s="12" t="n"/>
-      <c r="L29" s="12" t="n"/>
-      <c r="M29" s="12" t="inlineStr"/>
-      <c r="N29" s="12" t="n"/>
-      <c r="O29" s="12" t="n"/>
-      <c r="P29" s="12" t="n"/>
-      <c r="Q29" s="12" t="n"/>
-      <c r="R29" s="12" t="n"/>
-      <c r="S29" s="12" t="n"/>
-      <c r="T29" s="12" t="n"/>
+      <c r="E29" s="16" t="n"/>
+      <c r="F29" s="16" t="n"/>
+      <c r="G29" s="16" t="inlineStr"/>
+      <c r="H29" s="16" t="inlineStr"/>
+      <c r="I29" s="16" t="inlineStr"/>
+      <c r="J29" s="16" t="inlineStr"/>
+      <c r="K29" s="16" t="n"/>
+      <c r="L29" s="16" t="n"/>
+      <c r="M29" s="16" t="n"/>
+      <c r="N29" s="16" t="n"/>
+      <c r="O29" s="16" t="n"/>
+      <c r="P29" s="16" t="n"/>
+      <c r="Q29" s="16" t="n"/>
+      <c r="R29" s="16" t="n"/>
+      <c r="S29" s="16" t="n"/>
+      <c r="T29" s="16" t="n"/>
     </row>
     <row r="30">
-      <c r="C30" s="12" t="inlineStr">
+      <c r="C30" s="16" t="inlineStr">
         <is>
           <t>systemFieldWidgetFg</t>
         </is>
       </c>
-      <c r="D30" s="12" t="inlineStr">
+      <c r="D30" s="16" t="inlineStr">
         <is>
           <t>table</t>
         </is>
       </c>
-      <c r="E30" s="12" t="inlineStr">
+      <c r="E30" s="16" t="inlineStr">
         <is>
           <t>System Field Widget</t>
         </is>
       </c>
-      <c r="F30" s="12" t="inlineStr">
+      <c r="F30" s="16" t="inlineStr">
         <is>
           <t>systemFieldWidgetRcs</t>
         </is>
       </c>
-      <c r="G30" s="12" t="inlineStr"/>
-      <c r="H30" s="12" t="inlineStr"/>
-      <c r="I30" s="12" t="inlineStr"/>
-      <c r="J30" s="12" t="inlineStr">
+      <c r="G30" s="16" t="inlineStr"/>
+      <c r="H30" s="16" t="inlineStr"/>
+      <c r="I30" s="16" t="inlineStr"/>
+      <c r="J30" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="K30" s="12" t="n"/>
-      <c r="L30" s="12" t="n"/>
-      <c r="M30" s="12" t="inlineStr"/>
-      <c r="N30" s="12" t="n"/>
-      <c r="O30" s="12" t="n"/>
-      <c r="P30" s="12" t="n"/>
-      <c r="Q30" s="12" t="n"/>
-      <c r="R30" s="12" t="n"/>
-      <c r="S30" s="12" t="n"/>
-      <c r="T30" s="12" t="n"/>
+      <c r="K30" s="16" t="n"/>
+      <c r="L30" s="16" t="n"/>
+      <c r="M30" s="16" t="n"/>
+      <c r="N30" s="16" t="n"/>
+      <c r="O30" s="16" t="n"/>
+      <c r="P30" s="16" t="n"/>
+      <c r="Q30" s="16" t="n"/>
+      <c r="R30" s="16" t="n"/>
+      <c r="S30" s="16" t="n"/>
+      <c r="T30" s="16" t="n"/>
     </row>
     <row r="31">
-      <c r="C31" s="12" t="inlineStr">
+      <c r="C31" s="16" t="inlineStr">
         <is>
           <t>customFieldWidgetFg</t>
         </is>
       </c>
-      <c r="D31" s="12" t="inlineStr">
+      <c r="D31" s="16" t="inlineStr">
         <is>
           <t>table</t>
         </is>
       </c>
-      <c r="E31" s="12" t="inlineStr">
+      <c r="E31" s="16" t="inlineStr">
         <is>
           <t>Custom Field Widget</t>
         </is>
       </c>
-      <c r="F31" s="12" t="inlineStr">
+      <c r="F31" s="16" t="inlineStr">
         <is>
           <t>customFieldWidgetRcs</t>
         </is>
       </c>
-      <c r="G31" s="12" t="inlineStr">
+      <c r="G31" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H31" s="12" t="inlineStr">
+      <c r="H31" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="I31" s="12" t="inlineStr">
+      <c r="I31" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="J31" s="12" t="inlineStr">
+      <c r="J31" s="16" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="K31" s="12" t="n"/>
-      <c r="L31" s="12" t="n"/>
-      <c r="M31" s="12" t="inlineStr"/>
-      <c r="N31" s="12" t="n"/>
-      <c r="O31" s="12" t="n"/>
-      <c r="P31" s="12" t="n"/>
-      <c r="Q31" s="12" t="n"/>
-      <c r="R31" s="12" t="n"/>
-      <c r="S31" s="12" t="n"/>
-      <c r="T31" s="12" t="n"/>
+      <c r="K31" s="16" t="n"/>
+      <c r="L31" s="16" t="n"/>
+      <c r="M31" s="16" t="n"/>
+      <c r="N31" s="16" t="n"/>
+      <c r="O31" s="16" t="n"/>
+      <c r="P31" s="16" t="n"/>
+      <c r="Q31" s="16" t="n"/>
+      <c r="R31" s="16" t="n"/>
+      <c r="S31" s="16" t="n"/>
+      <c r="T31" s="16" t="n"/>
     </row>
     <row r="32">
-      <c r="C32" s="12" t="inlineStr">
+      <c r="C32" s="16" t="inlineStr">
         <is>
           <t>fieldWidgetToolbar</t>
         </is>
       </c>
-      <c r="D32" s="12" t="inlineStr">
+      <c r="D32" s="16" t="inlineStr">
         <is>
           <t>iconBar</t>
         </is>
       </c>
-      <c r="E32" s="12" t="n"/>
-      <c r="F32" s="12" t="n"/>
-      <c r="G32" s="12" t="inlineStr"/>
-      <c r="H32" s="12" t="inlineStr"/>
-      <c r="I32" s="12" t="inlineStr"/>
-      <c r="J32" s="12" t="inlineStr"/>
-      <c r="K32" s="12" t="n"/>
-      <c r="L32" s="12" t="n"/>
-      <c r="M32" s="12" t="inlineStr"/>
-      <c r="N32" s="12" t="n"/>
-      <c r="O32" s="12" t="n"/>
-      <c r="P32" s="12" t="n"/>
-      <c r="Q32" s="12" t="n"/>
-      <c r="R32" s="12" t="n"/>
-      <c r="S32" s="12" t="n"/>
-      <c r="T32" s="12" t="n"/>
+      <c r="E32" s="16" t="n"/>
+      <c r="F32" s="16" t="n"/>
+      <c r="G32" s="16" t="inlineStr"/>
+      <c r="H32" s="16" t="inlineStr"/>
+      <c r="I32" s="16" t="inlineStr"/>
+      <c r="J32" s="16" t="inlineStr"/>
+      <c r="K32" s="16" t="n"/>
+      <c r="L32" s="16" t="n"/>
+      <c r="M32" s="16" t="n"/>
+      <c r="N32" s="16" t="n"/>
+      <c r="O32" s="16" t="n"/>
+      <c r="P32" s="16" t="n"/>
+      <c r="Q32" s="16" t="n"/>
+      <c r="R32" s="16" t="n"/>
+      <c r="S32" s="16" t="n"/>
+      <c r="T32" s="16" t="n"/>
     </row>
     <row r="33">
-      <c r="C33" s="5" t="inlineStr">
+      <c r="A33" s="11" t="n"/>
+      <c r="C33" s="9" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D33" s="3" t="n"/>
-      <c r="E33" s="3" t="n"/>
-      <c r="F33" s="3" t="n"/>
-      <c r="G33" s="3" t="n"/>
-      <c r="H33" s="3" t="n"/>
-      <c r="I33" s="3" t="n"/>
-      <c r="J33" s="3" t="n"/>
-      <c r="K33" s="3" t="n"/>
-      <c r="L33" s="3" t="n"/>
-      <c r="M33" s="3" t="n"/>
-      <c r="N33" s="3" t="n"/>
-      <c r="O33" s="3" t="n"/>
-      <c r="P33" s="3" t="n"/>
-      <c r="Q33" s="3" t="n"/>
-      <c r="R33" s="3" t="n"/>
-      <c r="S33" s="3" t="n"/>
-      <c r="T33" s="3" t="n"/>
+      <c r="D33" s="7" t="n"/>
+      <c r="E33" s="7" t="n"/>
+      <c r="F33" s="7" t="n"/>
+      <c r="G33" s="7" t="n"/>
+      <c r="H33" s="7" t="n"/>
+      <c r="I33" s="7" t="n"/>
+      <c r="J33" s="7" t="n"/>
+      <c r="K33" s="7" t="n"/>
+      <c r="L33" s="7" t="n"/>
+      <c r="M33" s="7" t="n"/>
+      <c r="N33" s="7" t="n"/>
+      <c r="O33" s="7" t="n"/>
+      <c r="P33" s="7" t="n"/>
+      <c r="Q33" s="7" t="n"/>
+      <c r="R33" s="7" t="n"/>
+      <c r="S33" s="7" t="n"/>
+      <c r="T33" s="7" t="n"/>
     </row>
     <row r="34"/>
     <row r="35">
-      <c r="K35" s="9" t="n"/>
-      <c r="L35" s="13" t="inlineStr">
+      <c r="A35" s="11" t="n"/>
+      <c r="K35" s="13" t="n"/>
+      <c r="L35" s="17" t="inlineStr">
         <is>
           <t>Data type, Data Length, Required should come from model</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="C36" s="9" t="n"/>
-      <c r="D36" s="9" t="inlineStr">
+      <c r="A36" s="11" t="n"/>
+      <c r="C36" s="13" t="n"/>
+      <c r="D36" s="13" t="inlineStr">
         <is>
           <t>Python Name</t>
         </is>
       </c>
-      <c r="E36" s="9" t="n"/>
-      <c r="F36" s="9" t="n"/>
-      <c r="G36" s="9" t="n"/>
-      <c r="H36" s="11" t="inlineStr">
+      <c r="E36" s="13" t="n"/>
+      <c r="F36" s="13" t="n"/>
+      <c r="G36" s="13" t="n"/>
+      <c r="H36" s="15" t="inlineStr">
         <is>
           <t>( blank / no  )</t>
         </is>
       </c>
-      <c r="I36" s="11" t="inlineStr">
+      <c r="I36" s="15" t="inlineStr">
         <is>
           <t>e.g. textbox</t>
         </is>
       </c>
-      <c r="K36" s="17" t="n"/>
-      <c r="L36" s="21" t="inlineStr">
+      <c r="K36" s="21" t="n"/>
+      <c r="L36" s="25" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="M36" s="20" t="n"/>
+      <c r="M36" s="24" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="7" t="inlineStr">
+      <c r="A37" s="11" t="inlineStr">
         <is>
           <t>fieldTable</t>
         </is>
       </c>
-      <c r="B37" s="1" t="inlineStr">
+      <c r="B37" s="5" t="inlineStr">
         <is>
           <t>Fields</t>
         </is>
       </c>
-      <c r="C37" s="3" t="inlineStr">
+      <c r="C37" s="7" t="inlineStr">
         <is>
           <t>Field Group Name</t>
         </is>
       </c>
-      <c r="D37" s="3" t="inlineStr">
+      <c r="D37" s="7" t="inlineStr">
         <is>
           <t>Field Name</t>
         </is>
       </c>
-      <c r="E37" s="3" t="inlineStr">
+      <c r="E37" s="7" t="inlineStr">
         <is>
           <t>Caption</t>
         </is>
       </c>
-      <c r="F37" s="3" t="inlineStr">
+      <c r="F37" s="7" t="inlineStr">
         <is>
           <t>Tooltip</t>
         </is>
       </c>
-      <c r="G37" s="3" t="inlineStr">
+      <c r="G37" s="7" t="inlineStr">
         <is>
           <t>Hidden</t>
         </is>
       </c>
-      <c r="H37" s="3" t="inlineStr">
+      <c r="H37" s="7" t="inlineStr">
         <is>
           <t>Editable</t>
         </is>
       </c>
-      <c r="I37" s="3" t="inlineStr">
+      <c r="I37" s="7" t="inlineStr">
         <is>
           <t>Widget</t>
         </is>
       </c>
-      <c r="J37" s="3" t="inlineStr">
+      <c r="J37" s="7" t="inlineStr">
         <is>
           <t>Widget Parameters</t>
         </is>
       </c>
-      <c r="K37" s="10" t="inlineStr">
+      <c r="K37" s="14" t="inlineStr">
         <is>
           <t>Field</t>
         </is>
       </c>
-      <c r="L37" s="3" t="inlineStr">
+      <c r="L37" s="7" t="inlineStr">
         <is>
           <t>Format</t>
         </is>
       </c>
-      <c r="M37" s="3" t="inlineStr">
+      <c r="M37" s="7" t="inlineStr">
         <is>
           <t>Validation</t>
         </is>
       </c>
-      <c r="N37" s="3" t="inlineStr">
+      <c r="N37" s="7" t="inlineStr">
         <is>
           <t>Event Handler</t>
         </is>
       </c>
-      <c r="O37" s="3" t="inlineStr">
+      <c r="O37" s="7" t="inlineStr">
         <is>
           <t>Styles</t>
         </is>
       </c>
-      <c r="P37" s="3" t="inlineStr">
+      <c r="P37" s="7" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="1" t="n"/>
-      <c r="C38" s="12" t="inlineStr">
+      <c r="A38" s="11" t="n"/>
+      <c r="B38" s="5" t="n"/>
+      <c r="C38" s="16" t="inlineStr">
         <is>
           <t>systemFgTypeFg</t>
         </is>
       </c>
-      <c r="D38" s="12" t="inlineStr">
+      <c r="D38" s="16" t="inlineStr">
         <is>
           <t>sysTpNm</t>
         </is>
       </c>
-      <c r="E38" s="12" t="inlineStr">
+      <c r="E38" s="16" t="inlineStr">
         <is>
           <t>Type Name</t>
         </is>
       </c>
-      <c r="F38" s="12" t="n"/>
-      <c r="G38" s="12" t="inlineStr"/>
-      <c r="H38" s="12" t="inlineStr"/>
-      <c r="I38" s="12" t="inlineStr">
+      <c r="F38" s="16" t="n"/>
+      <c r="G38" s="16" t="inlineStr"/>
+      <c r="H38" s="16" t="inlineStr"/>
+      <c r="I38" s="16" t="inlineStr">
         <is>
           <t>Label</t>
         </is>
       </c>
-      <c r="J38" s="12" t="n"/>
-      <c r="K38" s="12" t="inlineStr">
+      <c r="J38" s="16" t="n"/>
+      <c r="K38" s="16" t="inlineStr">
         <is>
           <t>type_nm</t>
         </is>
       </c>
-      <c r="L38" s="12" t="n"/>
-      <c r="M38" s="12" t="n"/>
-      <c r="N38" s="12" t="n"/>
-      <c r="O38" s="12" t="n"/>
-      <c r="P38" s="12" t="n"/>
+      <c r="L38" s="16" t="n"/>
+      <c r="M38" s="16" t="n"/>
+      <c r="N38" s="16" t="n"/>
+      <c r="O38" s="16" t="n"/>
+      <c r="P38" s="16" t="n"/>
     </row>
     <row r="39">
-      <c r="C39" s="12" t="inlineStr"/>
-      <c r="D39" s="12" t="inlineStr">
+      <c r="C39" s="16" t="inlineStr"/>
+      <c r="D39" s="16" t="inlineStr">
         <is>
           <t>sysTpRmk</t>
         </is>
       </c>
-      <c r="E39" s="12" t="inlineStr">
+      <c r="E39" s="16" t="inlineStr">
         <is>
           <t>Remark</t>
         </is>
       </c>
-      <c r="F39" s="12" t="n"/>
-      <c r="G39" s="12" t="inlineStr"/>
-      <c r="H39" s="12" t="inlineStr"/>
-      <c r="I39" s="12" t="inlineStr">
+      <c r="F39" s="16" t="n"/>
+      <c r="G39" s="16" t="inlineStr"/>
+      <c r="H39" s="16" t="inlineStr"/>
+      <c r="I39" s="16" t="inlineStr">
         <is>
           <t>Label</t>
         </is>
       </c>
-      <c r="J39" s="12" t="n"/>
-      <c r="K39" s="12" t="inlineStr">
+      <c r="J39" s="16" t="n"/>
+      <c r="K39" s="16" t="inlineStr">
         <is>
           <t>rmk</t>
         </is>
       </c>
-      <c r="L39" s="12" t="n"/>
-      <c r="M39" s="12" t="n"/>
-      <c r="N39" s="12" t="n"/>
-      <c r="O39" s="12" t="n"/>
-      <c r="P39" s="12" t="n"/>
+      <c r="L39" s="16" t="n"/>
+      <c r="M39" s="16" t="n"/>
+      <c r="N39" s="16" t="n"/>
+      <c r="O39" s="16" t="n"/>
+      <c r="P39" s="16" t="n"/>
     </row>
     <row r="40">
-      <c r="C40" s="12" t="inlineStr">
+      <c r="C40" s="16" t="inlineStr">
         <is>
           <t>customFgTypeFg</t>
         </is>
       </c>
-      <c r="D40" s="12" t="inlineStr">
+      <c r="D40" s="16" t="inlineStr">
         <is>
           <t>customTpNm</t>
         </is>
       </c>
-      <c r="E40" s="12" t="inlineStr">
+      <c r="E40" s="16" t="inlineStr">
         <is>
           <t>Type Name</t>
         </is>
       </c>
-      <c r="F40" s="12" t="n"/>
-      <c r="G40" s="12" t="inlineStr"/>
-      <c r="H40" s="12" t="inlineStr"/>
-      <c r="I40" s="12" t="inlineStr">
+      <c r="F40" s="16" t="n"/>
+      <c r="G40" s="16" t="inlineStr"/>
+      <c r="H40" s="16" t="inlineStr"/>
+      <c r="I40" s="16" t="inlineStr">
         <is>
           <t>TextBox</t>
         </is>
       </c>
-      <c r="J40" s="12" t="n"/>
-      <c r="K40" s="12" t="inlineStr">
+      <c r="J40" s="16" t="n"/>
+      <c r="K40" s="16" t="inlineStr">
         <is>
           <t>type_nm</t>
         </is>
       </c>
-      <c r="L40" s="12" t="n"/>
-      <c r="M40" s="12" t="n"/>
-      <c r="N40" s="12" t="n"/>
-      <c r="O40" s="12" t="n"/>
-      <c r="P40" s="12" t="n"/>
+      <c r="L40" s="16" t="n"/>
+      <c r="M40" s="16" t="n"/>
+      <c r="N40" s="16" t="n"/>
+      <c r="O40" s="16" t="n"/>
+      <c r="P40" s="16" t="n"/>
     </row>
     <row r="41">
-      <c r="C41" s="12" t="inlineStr"/>
-      <c r="D41" s="12" t="inlineStr">
+      <c r="C41" s="16" t="inlineStr"/>
+      <c r="D41" s="16" t="inlineStr">
         <is>
           <t>customTpRmk</t>
         </is>
       </c>
-      <c r="E41" s="12" t="inlineStr">
+      <c r="E41" s="16" t="inlineStr">
         <is>
           <t>Remark</t>
         </is>
       </c>
-      <c r="F41" s="12" t="n"/>
-      <c r="G41" s="12" t="inlineStr"/>
-      <c r="H41" s="12" t="inlineStr"/>
-      <c r="I41" s="12" t="inlineStr">
+      <c r="F41" s="16" t="n"/>
+      <c r="G41" s="16" t="inlineStr"/>
+      <c r="H41" s="16" t="inlineStr"/>
+      <c r="I41" s="16" t="inlineStr">
         <is>
           <t>TextBox</t>
         </is>
       </c>
-      <c r="J41" s="12" t="n"/>
-      <c r="K41" s="12" t="inlineStr">
+      <c r="J41" s="16" t="n"/>
+      <c r="K41" s="16" t="inlineStr">
         <is>
           <t>rmk</t>
         </is>
       </c>
-      <c r="L41" s="12" t="n"/>
-      <c r="M41" s="12" t="n"/>
-      <c r="N41" s="12" t="n"/>
-      <c r="O41" s="12" t="n"/>
-      <c r="P41" s="12" t="n"/>
+      <c r="L41" s="16" t="n"/>
+      <c r="M41" s="16" t="n"/>
+      <c r="N41" s="16" t="n"/>
+      <c r="O41" s="16" t="n"/>
+      <c r="P41" s="16" t="n"/>
     </row>
     <row r="42">
-      <c r="C42" s="12" t="inlineStr">
+      <c r="C42" s="16" t="inlineStr">
         <is>
           <t>fgTypeToolbar</t>
         </is>
       </c>
-      <c r="D42" s="12" t="inlineStr">
+      <c r="D42" s="16" t="inlineStr">
         <is>
           <t>bttSaveTp</t>
         </is>
       </c>
-      <c r="E42" s="12" t="inlineStr">
+      <c r="E42" s="16" t="inlineStr">
         <is>
           <t>Save Field Group Type</t>
         </is>
       </c>
-      <c r="F42" s="12" t="n"/>
-      <c r="G42" s="12" t="inlineStr"/>
-      <c r="H42" s="12" t="inlineStr"/>
-      <c r="I42" s="12" t="inlineStr">
+      <c r="F42" s="16" t="n"/>
+      <c r="G42" s="16" t="inlineStr"/>
+      <c r="H42" s="16" t="inlineStr"/>
+      <c r="I42" s="16" t="inlineStr">
         <is>
           <t>IconAndText</t>
         </is>
       </c>
-      <c r="J42" s="12" t="inlineStr">
+      <c r="J42" s="16" t="inlineStr">
         <is>
           <t>icon:images/save_button.gif</t>
         </is>
       </c>
-      <c r="K42" s="12" t="n"/>
-      <c r="L42" s="12" t="n"/>
-      <c r="M42" s="12" t="n"/>
-      <c r="N42" s="12" t="inlineStr">
+      <c r="K42" s="16" t="n"/>
+      <c r="L42" s="16" t="n"/>
+      <c r="M42" s="16" t="n"/>
+      <c r="N42" s="16" t="inlineStr">
         <is>
           <t>saveFgType(customFgTypeFg)</t>
         </is>
       </c>
-      <c r="O42" s="12" t="n"/>
-      <c r="P42" s="12" t="n"/>
+      <c r="O42" s="16" t="n"/>
+      <c r="P42" s="16" t="n"/>
     </row>
     <row r="43">
-      <c r="C43" s="12" t="inlineStr">
+      <c r="C43" s="16" t="inlineStr">
         <is>
           <t>systemFieldWidgetFg</t>
         </is>
       </c>
-      <c r="D43" s="12" t="inlineStr">
+      <c r="D43" s="16" t="inlineStr">
         <is>
           <t>sysWidgetNm</t>
         </is>
       </c>
-      <c r="E43" s="12" t="inlineStr">
+      <c r="E43" s="16" t="inlineStr">
         <is>
           <t>Widget Name</t>
         </is>
       </c>
-      <c r="F43" s="12" t="n"/>
-      <c r="G43" s="12" t="inlineStr"/>
-      <c r="H43" s="12" t="inlineStr"/>
-      <c r="I43" s="12" t="inlineStr">
+      <c r="F43" s="16" t="n"/>
+      <c r="G43" s="16" t="inlineStr"/>
+      <c r="H43" s="16" t="inlineStr"/>
+      <c r="I43" s="16" t="inlineStr">
         <is>
           <t>Label</t>
         </is>
       </c>
-      <c r="J43" s="12" t="n"/>
-      <c r="K43" s="12" t="inlineStr">
+      <c r="J43" s="16" t="n"/>
+      <c r="K43" s="16" t="inlineStr">
         <is>
           <t>widget_nm</t>
         </is>
       </c>
-      <c r="L43" s="12" t="n"/>
-      <c r="M43" s="12" t="n"/>
-      <c r="N43" s="12" t="n"/>
-      <c r="O43" s="12" t="n"/>
-      <c r="P43" s="12" t="n"/>
+      <c r="L43" s="16" t="n"/>
+      <c r="M43" s="16" t="n"/>
+      <c r="N43" s="16" t="n"/>
+      <c r="O43" s="16" t="n"/>
+      <c r="P43" s="16" t="n"/>
     </row>
     <row r="44">
-      <c r="C44" s="12" t="inlineStr"/>
-      <c r="D44" s="12" t="inlineStr">
+      <c r="C44" s="16" t="inlineStr"/>
+      <c r="D44" s="16" t="inlineStr">
         <is>
           <t>sysWidgetRmk</t>
         </is>
       </c>
-      <c r="E44" s="12" t="inlineStr">
+      <c r="E44" s="16" t="inlineStr">
         <is>
           <t>Remark</t>
         </is>
       </c>
-      <c r="F44" s="12" t="n"/>
-      <c r="G44" s="12" t="inlineStr"/>
-      <c r="H44" s="12" t="inlineStr"/>
-      <c r="I44" s="12" t="inlineStr">
+      <c r="F44" s="16" t="n"/>
+      <c r="G44" s="16" t="inlineStr"/>
+      <c r="H44" s="16" t="inlineStr"/>
+      <c r="I44" s="16" t="inlineStr">
         <is>
           <t>Label</t>
         </is>
       </c>
-      <c r="J44" s="12" t="n"/>
-      <c r="K44" s="12" t="inlineStr">
+      <c r="J44" s="16" t="n"/>
+      <c r="K44" s="16" t="inlineStr">
         <is>
           <t>rmk</t>
         </is>
       </c>
-      <c r="L44" s="12" t="n"/>
-      <c r="M44" s="12" t="n"/>
-      <c r="N44" s="12" t="n"/>
-      <c r="O44" s="12" t="n"/>
-      <c r="P44" s="12" t="n"/>
+      <c r="L44" s="16" t="n"/>
+      <c r="M44" s="16" t="n"/>
+      <c r="N44" s="16" t="n"/>
+      <c r="O44" s="16" t="n"/>
+      <c r="P44" s="16" t="n"/>
     </row>
     <row r="45">
-      <c r="C45" s="12" t="inlineStr">
+      <c r="C45" s="16" t="inlineStr">
         <is>
           <t>customFieldWidgetFg</t>
         </is>
       </c>
-      <c r="D45" s="12" t="inlineStr">
+      <c r="D45" s="16" t="inlineStr">
         <is>
           <t>customWidgetNm</t>
         </is>
       </c>
-      <c r="E45" s="12" t="inlineStr">
+      <c r="E45" s="16" t="inlineStr">
         <is>
           <t>Widget Name</t>
         </is>
       </c>
-      <c r="F45" s="12" t="n"/>
-      <c r="G45" s="12" t="inlineStr"/>
-      <c r="H45" s="12" t="inlineStr"/>
-      <c r="I45" s="12" t="inlineStr">
+      <c r="F45" s="16" t="n"/>
+      <c r="G45" s="16" t="inlineStr"/>
+      <c r="H45" s="16" t="inlineStr"/>
+      <c r="I45" s="16" t="inlineStr">
         <is>
           <t>TextBox</t>
         </is>
       </c>
-      <c r="J45" s="12" t="n"/>
-      <c r="K45" s="12" t="inlineStr">
+      <c r="J45" s="16" t="n"/>
+      <c r="K45" s="16" t="inlineStr">
         <is>
           <t>widget_nm</t>
         </is>
       </c>
-      <c r="L45" s="12" t="n"/>
-      <c r="M45" s="12" t="n"/>
-      <c r="N45" s="12" t="n"/>
-      <c r="O45" s="12" t="n"/>
-      <c r="P45" s="12" t="n"/>
+      <c r="L45" s="16" t="n"/>
+      <c r="M45" s="16" t="n"/>
+      <c r="N45" s="16" t="n"/>
+      <c r="O45" s="16" t="n"/>
+      <c r="P45" s="16" t="n"/>
     </row>
     <row r="46">
-      <c r="C46" s="12" t="inlineStr"/>
-      <c r="D46" s="12" t="inlineStr">
+      <c r="C46" s="16" t="inlineStr"/>
+      <c r="D46" s="16" t="inlineStr">
         <is>
           <t>customWidgetRmk</t>
         </is>
       </c>
-      <c r="E46" s="12" t="inlineStr">
+      <c r="E46" s="16" t="inlineStr">
         <is>
           <t>Remark</t>
         </is>
       </c>
-      <c r="F46" s="12" t="n"/>
-      <c r="G46" s="12" t="inlineStr"/>
-      <c r="H46" s="12" t="inlineStr"/>
-      <c r="I46" s="12" t="inlineStr">
+      <c r="F46" s="16" t="n"/>
+      <c r="G46" s="16" t="inlineStr"/>
+      <c r="H46" s="16" t="inlineStr"/>
+      <c r="I46" s="16" t="inlineStr">
         <is>
           <t>TextBox</t>
         </is>
       </c>
-      <c r="J46" s="12" t="n"/>
-      <c r="K46" s="12" t="inlineStr">
+      <c r="J46" s="16" t="n"/>
+      <c r="K46" s="16" t="inlineStr">
         <is>
           <t>rmk</t>
         </is>
       </c>
-      <c r="L46" s="12" t="n"/>
-      <c r="M46" s="12" t="n"/>
-      <c r="N46" s="12" t="n"/>
-      <c r="O46" s="12" t="n"/>
-      <c r="P46" s="12" t="n"/>
+      <c r="L46" s="16" t="n"/>
+      <c r="M46" s="16" t="n"/>
+      <c r="N46" s="16" t="n"/>
+      <c r="O46" s="16" t="n"/>
+      <c r="P46" s="16" t="n"/>
     </row>
     <row r="47">
-      <c r="C47" s="12" t="inlineStr">
+      <c r="C47" s="16" t="inlineStr">
         <is>
           <t>fieldWidgetToolbar</t>
         </is>
       </c>
-      <c r="D47" s="12" t="inlineStr">
+      <c r="D47" s="16" t="inlineStr">
         <is>
           <t>bttSaveWidget</t>
         </is>
       </c>
-      <c r="E47" s="12" t="inlineStr">
+      <c r="E47" s="16" t="inlineStr">
         <is>
           <t>Save Field Widget</t>
         </is>
       </c>
-      <c r="F47" s="12" t="n"/>
-      <c r="G47" s="12" t="inlineStr"/>
-      <c r="H47" s="12" t="inlineStr"/>
-      <c r="I47" s="12" t="inlineStr">
+      <c r="F47" s="16" t="n"/>
+      <c r="G47" s="16" t="inlineStr"/>
+      <c r="H47" s="16" t="inlineStr"/>
+      <c r="I47" s="16" t="inlineStr">
         <is>
           <t>IconAndText</t>
         </is>
       </c>
-      <c r="J47" s="12" t="inlineStr">
+      <c r="J47" s="16" t="inlineStr">
         <is>
           <t>icon:images/save_button.gif</t>
         </is>
       </c>
-      <c r="K47" s="12" t="n"/>
-      <c r="L47" s="12" t="n"/>
-      <c r="M47" s="12" t="n"/>
-      <c r="N47" s="12" t="inlineStr">
+      <c r="K47" s="16" t="n"/>
+      <c r="L47" s="16" t="n"/>
+      <c r="M47" s="16" t="n"/>
+      <c r="N47" s="16" t="inlineStr">
         <is>
           <t>saveWidget(customFieldWidgetFg)</t>
         </is>
       </c>
-      <c r="O47" s="12" t="n"/>
-      <c r="P47" s="12" t="n"/>
+      <c r="O47" s="16" t="n"/>
+      <c r="P47" s="16" t="n"/>
     </row>
     <row r="48">
-      <c r="C48" s="5" t="inlineStr">
+      <c r="A48" s="11" t="n"/>
+      <c r="C48" s="9" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D48" s="3" t="n"/>
-      <c r="E48" s="3" t="n"/>
-      <c r="F48" s="3" t="n"/>
-      <c r="G48" s="3" t="n"/>
-      <c r="H48" s="3" t="n"/>
-      <c r="I48" s="3" t="n"/>
-      <c r="J48" s="3" t="n"/>
-      <c r="K48" s="3" t="n"/>
-      <c r="L48" s="3" t="n"/>
-      <c r="M48" s="3" t="n"/>
-      <c r="N48" s="3" t="n"/>
-      <c r="O48" s="3" t="n"/>
-      <c r="P48" s="3" t="n"/>
+      <c r="D48" s="7" t="n"/>
+      <c r="E48" s="7" t="n"/>
+      <c r="F48" s="7" t="n"/>
+      <c r="G48" s="7" t="n"/>
+      <c r="H48" s="7" t="n"/>
+      <c r="I48" s="7" t="n"/>
+      <c r="J48" s="7" t="n"/>
+      <c r="K48" s="7" t="n"/>
+      <c r="L48" s="7" t="n"/>
+      <c r="M48" s="7" t="n"/>
+      <c r="N48" s="7" t="n"/>
+      <c r="O48" s="7" t="n"/>
+      <c r="P48" s="7" t="n"/>
     </row>
     <row r="49"/>
     <row r="50"/>
     <row r="51"/>
     <row r="52">
-      <c r="A52" s="7" t="inlineStr">
+      <c r="A52" s="11" t="inlineStr">
         <is>
           <t>subScreenTable</t>
         </is>
       </c>
-      <c r="B52" s="1" t="inlineStr">
+      <c r="B52" s="5" t="inlineStr">
         <is>
           <t>Sub Screen</t>
         </is>
       </c>
-      <c r="C52" s="3" t="inlineStr">
+      <c r="C52" s="7" t="inlineStr">
         <is>
           <t>Sub Screen Name</t>
         </is>
       </c>
-      <c r="D52" s="3" t="inlineStr">
+      <c r="D52" s="7" t="inlineStr">
         <is>
           <t>Field Groups</t>
         </is>
       </c>
-      <c r="E52" s="3" t="inlineStr">
+      <c r="E52" s="7" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="C53" s="12" t="n"/>
-      <c r="D53" s="12" t="n"/>
-      <c r="E53" s="12" t="n"/>
+      <c r="A53" s="11" t="n"/>
+      <c r="C53" s="16" t="n"/>
+      <c r="D53" s="16" t="n"/>
+      <c r="E53" s="16" t="n"/>
     </row>
     <row r="54">
-      <c r="C54" s="5" t="inlineStr">
+      <c r="A54" s="11" t="n"/>
+      <c r="C54" s="9" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D54" s="3" t="n"/>
-      <c r="E54" s="3" t="n"/>
+      <c r="D54" s="7" t="n"/>
+      <c r="E54" s="7" t="n"/>
     </row>
     <row r="55"/>
-    <row r="56"/>
+    <row r="56">
+      <c r="A56" s="11" t="n"/>
+    </row>
     <row r="57">
-      <c r="B57" s="1" t="n"/>
+      <c r="A57" s="11" t="n"/>
+      <c r="B57" s="5" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="7" t="inlineStr">
+      <c r="A58" s="11" t="inlineStr">
         <is>
           <t>fieldGroupLinkTable</t>
         </is>
       </c>
-      <c r="B58" s="1" t="inlineStr">
+      <c r="B58" s="5" t="inlineStr">
         <is>
           <t>Field Group Links</t>
         </is>
       </c>
-      <c r="C58" s="3" t="inlineStr">
+      <c r="C58" s="7" t="inlineStr">
         <is>
           <t>Field Group Name</t>
         </is>
       </c>
-      <c r="D58" s="3" t="inlineStr">
+      <c r="D58" s="7" t="inlineStr">
         <is>
           <t>Local Key</t>
         </is>
       </c>
-      <c r="E58" s="3" t="inlineStr">
+      <c r="E58" s="7" t="inlineStr">
         <is>
           <t>Parent Field Group Name</t>
         </is>
       </c>
-      <c r="F58" s="3" t="inlineStr">
+      <c r="F58" s="7" t="inlineStr">
         <is>
           <t>Parent Key</t>
         </is>
       </c>
-      <c r="G58" s="3" t="inlineStr">
+      <c r="G58" s="7" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="C59" s="12" t="n"/>
-      <c r="D59" s="12" t="n"/>
-      <c r="E59" s="12" t="n"/>
-      <c r="F59" s="12" t="n"/>
-      <c r="G59" s="12" t="n"/>
+      <c r="A59" s="11" t="n"/>
+      <c r="C59" s="16" t="n"/>
+      <c r="D59" s="16" t="n"/>
+      <c r="E59" s="16" t="n"/>
+      <c r="F59" s="16" t="n"/>
+      <c r="G59" s="16" t="n"/>
     </row>
     <row r="60">
-      <c r="C60" s="5" t="inlineStr">
+      <c r="A60" s="11" t="n"/>
+      <c r="C60" s="9" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D60" s="3" t="n"/>
-      <c r="E60" s="3" t="n"/>
-      <c r="F60" s="3" t="n"/>
-      <c r="G60" s="3" t="n"/>
+      <c r="D60" s="7" t="n"/>
+      <c r="E60" s="7" t="n"/>
+      <c r="F60" s="7" t="n"/>
+      <c r="G60" s="7" t="n"/>
     </row>
     <row r="61"/>
     <row r="62"/>
     <row r="63">
-      <c r="B63" s="18" t="inlineStr">
+      <c r="A63" s="11" t="n"/>
+      <c r="B63" s="22" t="inlineStr">
         <is>
           <t>Table Header and Footer for Field Groups</t>
         </is>
       </c>
-      <c r="E63" s="8" t="inlineStr">
+      <c r="E63" s="12" t="inlineStr">
         <is>
           <t>add as many levels as needed</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="14" t="inlineStr">
+      <c r="A64" s="18" t="inlineStr">
         <is>
           <t>headerFooterTable</t>
         </is>
       </c>
-      <c r="B64" s="15" t="n"/>
-      <c r="C64" s="19" t="inlineStr">
+      <c r="B64" s="19" t="n"/>
+      <c r="C64" s="23" t="inlineStr">
         <is>
           <t>Field Group Name</t>
         </is>
       </c>
-      <c r="D64" s="19" t="inlineStr">
+      <c r="D64" s="23" t="inlineStr">
         <is>
           <t>Field</t>
         </is>
       </c>
-      <c r="E64" s="19" t="inlineStr">
+      <c r="E64" s="23" t="inlineStr">
         <is>
           <t>Header Level 1</t>
         </is>
       </c>
-      <c r="F64" s="19" t="inlineStr">
+      <c r="F64" s="23" t="inlineStr">
         <is>
           <t>Header Level 2</t>
         </is>
       </c>
-      <c r="G64" s="19" t="inlineStr">
+      <c r="G64" s="23" t="inlineStr">
         <is>
           <t>Header Level 3</t>
         </is>
       </c>
-      <c r="H64" s="19" t="inlineStr">
+      <c r="H64" s="23" t="inlineStr">
         <is>
           <t>Footer</t>
         </is>
       </c>
-      <c r="I64" s="19" t="inlineStr">
+      <c r="I64" s="23" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
-      <c r="K64" s="8" t="inlineStr">
+      <c r="K64" s="12" t="inlineStr">
         <is>
           <t>optional for table field groups only</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="C65" s="12" t="n"/>
-      <c r="D65" s="12" t="n"/>
-      <c r="E65" s="12" t="n"/>
-      <c r="F65" s="12" t="n"/>
-      <c r="G65" s="12" t="n"/>
-      <c r="H65" s="12" t="n"/>
-      <c r="I65" s="12" t="n"/>
-      <c r="K65" s="8" t="inlineStr">
+      <c r="A65" s="11" t="n"/>
+      <c r="C65" s="16" t="n"/>
+      <c r="D65" s="16" t="n"/>
+      <c r="E65" s="16" t="n"/>
+      <c r="F65" s="16" t="n"/>
+      <c r="G65" s="16" t="n"/>
+      <c r="H65" s="16" t="n"/>
+      <c r="I65" s="16" t="n"/>
+      <c r="K65" s="12" t="inlineStr">
         <is>
           <t>this is only an example, does not match the above definition</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="C66" s="5" t="inlineStr">
+      <c r="C66" s="9" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D66" s="3" t="n"/>
-      <c r="E66" s="3" t="n"/>
-      <c r="F66" s="3" t="n"/>
-      <c r="G66" s="3" t="n"/>
-      <c r="H66" s="3" t="n"/>
-      <c r="I66" s="3" t="n"/>
+      <c r="D66" s="7" t="n"/>
+      <c r="E66" s="7" t="n"/>
+      <c r="F66" s="7" t="n"/>
+      <c r="G66" s="7" t="n"/>
+      <c r="H66" s="7" t="n"/>
+      <c r="I66" s="7" t="n"/>
     </row>
     <row r="67">
-      <c r="H67" s="8" t="n"/>
+      <c r="H67" s="12" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2656,7 +2680,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12.7109375" customWidth="1" min="1" max="1"/>
+    <col width="12.7109375" customWidth="1" style="4" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -2666,7 +2690,7 @@
           <t>Layout Type</t>
         </is>
       </c>
-      <c r="C5" s="8" t="inlineStr">
+      <c r="C5" s="12" t="inlineStr">
         <is>
           <t>One tailor made javascript for each layout</t>
         </is>

</xml_diff>